<commit_message>
new textbook xlsx files
</commit_message>
<xml_diff>
--- a/usatutor_admin/textbook_admin/usatutor_textbook.xlsx
+++ b/usatutor_admin/textbook_admin/usatutor_textbook.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\我的库\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF50D7B-AD9B-4949-9189-1BFEFA55D8B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D58124BA-A942-453D-9DE3-4192D13FA525}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="435" windowWidth="14400" windowHeight="8250" xr2:uid="{16D8FE33-4673-44B1-A48F-F5A13B792293}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640" xr2:uid="{16D8FE33-4673-44B1-A48F-F5A13B792293}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="342">
   <si>
     <t>level1</t>
   </si>
@@ -911,277 +912,397 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>https://ibb.co/c27p8KJ</t>
-  </si>
-  <si>
-    <t>https://ibb.co/MBVCCcL</t>
-  </si>
-  <si>
-    <t>https://ibb.co/RTcSr2V</t>
-  </si>
-  <si>
-    <t>https://ibb.co/Dr8ZcFG</t>
-  </si>
-  <si>
-    <t>https://ibb.co/fQG0jwZ</t>
-  </si>
-  <si>
-    <t>https://ibb.co/SynnLmb</t>
-  </si>
-  <si>
-    <t>https://ibb.co/h9QXrsJ</t>
-  </si>
-  <si>
-    <t>https://ibb.co/F8N2NGR</t>
-  </si>
-  <si>
-    <t>https://ibb.co/7XyJYNH</t>
-  </si>
-  <si>
-    <t>https://ibb.co/M7nV1CK</t>
-  </si>
-  <si>
-    <t>https://ibb.co/N9v4FWL</t>
-  </si>
-  <si>
-    <t>https://ibb.co/vwqBT54</t>
-  </si>
-  <si>
-    <t>https://ibb.co/4dRJVcd</t>
-  </si>
-  <si>
-    <t>https://ibb.co/sQF1Wgq</t>
-  </si>
-  <si>
-    <t>https://ibb.co/hB0LQDz</t>
-  </si>
-  <si>
-    <t>https://ibb.co/GdcS7tR</t>
-  </si>
-  <si>
-    <t>https://ibb.co/HCwZ510</t>
-  </si>
-  <si>
-    <t>https://ibb.co/Lh2dGqw</t>
-  </si>
-  <si>
-    <t>https://ibb.co/gMrRJm8</t>
-  </si>
-  <si>
-    <t>https://ibb.co/Ykg9J24</t>
-  </si>
-  <si>
-    <t>https://ibb.co/WB1gTJn</t>
-  </si>
-  <si>
-    <t>https://ibb.co/sCHc1zY</t>
-  </si>
-  <si>
-    <t>https://ibb.co/J2hjD7t</t>
-  </si>
-  <si>
-    <t>https://ibb.co/WPMBNLB</t>
-  </si>
-  <si>
-    <t>https://ibb.co/dKXgR0C</t>
-  </si>
-  <si>
-    <t>https://ibb.co/qswxVKP</t>
-  </si>
-  <si>
-    <t>https://ibb.co/w7R2yk1</t>
-  </si>
-  <si>
-    <t>https://ibb.co/nz2TxZF</t>
-  </si>
-  <si>
-    <t>https://ibb.co/bW5bspy</t>
-  </si>
-  <si>
-    <t>https://ibb.co/X7FVX6p</t>
-  </si>
-  <si>
-    <t>https://ibb.co/B6gZKP3</t>
-  </si>
-  <si>
-    <t>https://ibb.co/L9VHKyJ</t>
-  </si>
-  <si>
-    <t>https://ibb.co/Ykr2d7t</t>
-  </si>
-  <si>
-    <t>https://ibb.co/d2m4WY2</t>
-  </si>
-  <si>
-    <t>https://ibb.co/G5V2Cqj</t>
-  </si>
-  <si>
-    <t>https://ibb.co/Dg5JHtW</t>
-  </si>
-  <si>
-    <t>https://ibb.co/bBc8SS9</t>
-  </si>
-  <si>
-    <t>https://ibb.co/m4c7CrZ</t>
-  </si>
-  <si>
-    <t>https://ibb.co/m5WYtXP</t>
-  </si>
-  <si>
-    <t>https://ibb.co/c8mJG2f</t>
-  </si>
-  <si>
-    <t>https://ibb.co/pdN4VJ8</t>
-  </si>
-  <si>
-    <t>https://ibb.co/PxYPcBV</t>
-  </si>
-  <si>
-    <t>https://ibb.co/6YKbKt8</t>
-  </si>
-  <si>
-    <t>https://ibb.co/gR9WdzX</t>
-  </si>
-  <si>
-    <t>https://ibb.co/NSHXrvT</t>
-  </si>
-  <si>
-    <t>https://ibb.co/6F1W5sj</t>
-  </si>
-  <si>
-    <t>https://ibb.co/Fnw8xqR</t>
-  </si>
-  <si>
-    <t>https://ibb.co/RHNwFT9</t>
-  </si>
-  <si>
-    <t>https://ibb.co/s1bcVZh</t>
-  </si>
-  <si>
-    <t>https://ibb.co/chMWZ1S</t>
-  </si>
-  <si>
-    <t>https://ibb.co/XFsChnC</t>
-  </si>
-  <si>
-    <t>https://ibb.co/9TTWNJ7</t>
-  </si>
-  <si>
-    <t>https://ibb.co/q0YfLm9</t>
-  </si>
-  <si>
-    <t>https://ibb.co/1T2P0CG</t>
-  </si>
-  <si>
-    <t>https://ibb.co/Mpc6KDf</t>
-  </si>
-  <si>
-    <t>https://ibb.co/L9QwDx0</t>
-  </si>
-  <si>
-    <t>https://ibb.co/tCR8Zfh</t>
-  </si>
-  <si>
-    <t>https://ibb.co/rFKXzjw</t>
-  </si>
-  <si>
-    <t>https://ibb.co/9sVnBrY</t>
-  </si>
-  <si>
-    <t>https://ibb.co/yWvCsnL</t>
-  </si>
-  <si>
-    <t>https://ibb.co/86F8cVP</t>
-  </si>
-  <si>
-    <t>https://ibb.co/y6m0jZ9</t>
-  </si>
-  <si>
-    <t>https://ibb.co/zHKfqNp</t>
-  </si>
-  <si>
-    <t>https://ibb.co/cFsFV20</t>
-  </si>
-  <si>
-    <t>https://ibb.co/zPcsJw7</t>
-  </si>
-  <si>
-    <t>https://ibb.co/YWfPpft</t>
-  </si>
-  <si>
-    <t>https://ibb.co/yyRBByH</t>
-  </si>
-  <si>
-    <t>https://ibb.co/LRCRSQJ</t>
-  </si>
-  <si>
-    <t>https://ibb.co/n31cbhy</t>
-  </si>
-  <si>
-    <t>https://ibb.co/PmCp2xW</t>
-  </si>
-  <si>
-    <t>https://ibb.co/nzqzKhc</t>
-  </si>
-  <si>
-    <t>https://ibb.co/7XSzMgb</t>
-  </si>
-  <si>
-    <t>https://ibb.co/CBPmn6G</t>
-  </si>
-  <si>
-    <t>https://ibb.co/PQQsNg5</t>
-  </si>
-  <si>
-    <t>https://ibb.co/547MVGf</t>
-  </si>
-  <si>
-    <t>https://ibb.co/VwZxD6T</t>
-  </si>
-  <si>
-    <t>https://ibb.co/bPgL8xT</t>
-  </si>
-  <si>
-    <t>https://ibb.co/QQkXC6N</t>
-  </si>
-  <si>
-    <t>https://ibb.co/WWzPqpd</t>
-  </si>
-  <si>
-    <t>https://ibb.co/YQHz2gF</t>
-  </si>
-  <si>
-    <t>https://ibb.co/1RQRMCQ</t>
-  </si>
-  <si>
-    <t>https://ibb.co/Khb816T</t>
-  </si>
-  <si>
-    <t>https://ibb.co/SsWgVFw</t>
-  </si>
-  <si>
-    <t>https://ibb.co/qdGbHnj</t>
-  </si>
-  <si>
-    <t>https://ibb.co/2hkq8bS</t>
-  </si>
-  <si>
-    <t>https://ibb.co/c379KtV</t>
-  </si>
-  <si>
-    <t>https://ibb.co/2FQ2FBJ</t>
-  </si>
-  <si>
-    <t>https://ibb.co/jrFrXQY</t>
-  </si>
-  <si>
-    <t>https://ibb.co/Hq1n5cB</t>
-  </si>
-  <si>
-    <t>https://ibb.co/pKfcZyT</t>
+    <t>subject</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>classification</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Science</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Animals</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Butterflies</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>pic url</t>
+  </si>
+  <si>
+    <t>Classifying Animals</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fish</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Food Chain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Frogs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hibernation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insects</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plants</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>George Washington Carver</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Forests</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Parts of a Plant</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plant Adaptations</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plant Life Cycle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Trees</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Habitats</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Arctic Habitats</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Desert</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Freshwater Habitats</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Grasslands</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ocean Habitats</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rainforests</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Conservation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Extinct and Endangered Species</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Natural Resoutces</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduce,Reuse,Recycle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>url</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://i.ibb.co/wKFPcKB/1-1-2.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/PQDbh4D/1-1-3.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/GMV6rVk/1-1-4.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/6XR85G4/1-1-5.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/WHYYtdS/1-2-1.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/rMLFTJy/1-2-2.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/ygCFdqQ/1-2-3.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/6ZPHhRt/1-2-4.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/b27LjTm/1-2-5.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/MMfx4WR/1-3-1.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/hfJzn0K/1-3-2.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/nrCZsS0/1-3-3.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/pwpYwMg/1-3-4.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/Bnjs87Y/1-3-5.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/3r87rWv/1-4-1.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/5YV2Xmv/1-4-2.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/5jN9tSG/1-4-3.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/p3jrwQD/1-4-4.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/bNFTK4Y/1-4-5.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/xsrFRkP/1-5-1.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/wwWLMrt/1-5-2.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/09xrF9h/1-5-3.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/QHbkvQW/1-5-4.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/WyHzMhP/1-5-5.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/RPBvk8j/1-6-1.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/V2Zg9LC/1-6-2.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/F071jQp/1-6-3.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/16s6GS9/1-6-4.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/4MXN0tJ/1-6-5.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/FYqnx48/2-1-1.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/mykN40z/2-1-2.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/g6rgkKQ/2-1-3.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/b6MNXmn/2-1-4.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/Pj3csm7/2-1-5.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/yV0HnN9/2-2-1.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/PYNMFkv/2-2-2.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/nmT6rnw/2-2-3.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/g7n9g7G/2-2-4.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/J7y2S2D/2-2-5.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/pLKsk6y/2-3-1.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/Ykt4FRX/2-3-2.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/TgqgmyR/2-3-3.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/GkncspK/2-3-4.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/SPkC3yt/2-3-5.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/bbX73yT/2-4-1.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/MfSLX09/2-4-2.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/ZSFWPn8/2-4-3.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/w6csq6T/2-4-4.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/gwFdptz/2-4-5.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/W5yVqpK/2-5-1.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/YLHyhLD/2-5-2.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/qxx5GRJ/2-5-3.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/gz8z97R/2-5-4.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/9bK7mMQ/2-5-5.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/bPy6sZ9/2-6-1.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/JkdzNR3/2-6-2.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/tb1SfRc/2-6-3.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/WzPZFtX/2-6-4.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/wsJXVcH/2-6-5.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/m0TKyy2/3-1-1.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/NZZ5Wcn/3-1-2.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/zZL4wfq/3-1-3.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/1QwKTFK/3-1-4.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/Q9WH4jv/3-1-5.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/tP4b4DK/3-2-1.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/m51LQ9Q/3-2-2.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/Ps2CGhh/3-2-3.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/cbr0WBy/3-2-4.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/JrVbhyp/3-2-5.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/Lzc94fr/3-3-1.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/ngvsN6G/3-3-2.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/mTT0LbF/3-3-3.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/s6GhNC9/3-3-4.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/ZLzWw6G/3-3-5.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/WDL3nbV/3-4-1.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/8NV64Xk/3-4-2.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/0njMrdT/3-4-3.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/CVyL8ht/3-4-4.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/C1bC5ym/3-4-5.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/9Wwqm4m/3-5-1.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/KqZxSJ7/3-5-2.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/y5sjdZW/3-5-3.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/NTdKzHs/3-5-4.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/Zm3nVtf/3-5-5.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/68dhycT/3-6-1.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/w0WCLnX/3-6-2.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/D8GSTpr/3-6-3.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/d2NSrwy/3-6-4.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/FXng202/3-6-5.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/RTW172b/1-1-1.png</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1189,7 +1310,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1200,6 +1321,15 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
@@ -1229,21 +1359,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1558,7 +1698,7 @@
   <dimension ref="A1:F91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1566,7 +1706,7 @@
     <col min="3" max="3" width="17.125" customWidth="1"/>
     <col min="4" max="4" width="17.875" customWidth="1"/>
     <col min="5" max="5" width="36.375" customWidth="1"/>
-    <col min="6" max="6" width="22.75" customWidth="1"/>
+    <col min="6" max="6" width="33.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -1586,7 +1726,7 @@
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>311</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1605,8 +1745,8 @@
       <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
-        <v>221</v>
+      <c r="F2" s="3" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1626,7 +1766,7 @@
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>222</v>
+        <v>252</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1646,7 +1786,7 @@
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>223</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1666,7 +1806,7 @@
         <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>224</v>
+        <v>254</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1686,7 +1826,7 @@
         <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>225</v>
+        <v>255</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1706,7 +1846,7 @@
         <v>22</v>
       </c>
       <c r="F7" t="s">
-        <v>226</v>
+        <v>256</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1726,7 +1866,7 @@
         <v>24</v>
       </c>
       <c r="F8" t="s">
-        <v>227</v>
+        <v>257</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1746,7 +1886,7 @@
         <v>26</v>
       </c>
       <c r="F9" t="s">
-        <v>228</v>
+        <v>258</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1766,7 +1906,7 @@
         <v>28</v>
       </c>
       <c r="F10" t="s">
-        <v>229</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1786,7 +1926,7 @@
         <v>30</v>
       </c>
       <c r="F11" t="s">
-        <v>230</v>
+        <v>260</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1806,7 +1946,7 @@
         <v>35</v>
       </c>
       <c r="F12" t="s">
-        <v>231</v>
+        <v>261</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1826,7 +1966,7 @@
         <v>37</v>
       </c>
       <c r="F13" t="s">
-        <v>232</v>
+        <v>262</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1846,7 +1986,7 @@
         <v>39</v>
       </c>
       <c r="F14" t="s">
-        <v>233</v>
+        <v>263</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1866,7 +2006,7 @@
         <v>41</v>
       </c>
       <c r="F15" t="s">
-        <v>234</v>
+        <v>264</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1886,7 +2026,7 @@
         <v>43</v>
       </c>
       <c r="F16" t="s">
-        <v>235</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1906,7 +2046,7 @@
         <v>46</v>
       </c>
       <c r="F17" t="s">
-        <v>236</v>
+        <v>266</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1926,7 +2066,7 @@
         <v>48</v>
       </c>
       <c r="F18" t="s">
-        <v>237</v>
+        <v>267</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1946,7 +2086,7 @@
         <v>50</v>
       </c>
       <c r="F19" t="s">
-        <v>238</v>
+        <v>268</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1966,7 +2106,7 @@
         <v>52</v>
       </c>
       <c r="F20" t="s">
-        <v>239</v>
+        <v>269</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1986,7 +2126,7 @@
         <v>54</v>
       </c>
       <c r="F21" t="s">
-        <v>240</v>
+        <v>270</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -2006,7 +2146,7 @@
         <v>58</v>
       </c>
       <c r="F22" t="s">
-        <v>241</v>
+        <v>271</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -2026,7 +2166,7 @@
         <v>60</v>
       </c>
       <c r="F23" t="s">
-        <v>242</v>
+        <v>272</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -2046,7 +2186,7 @@
         <v>62</v>
       </c>
       <c r="F24" t="s">
-        <v>243</v>
+        <v>273</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -2066,7 +2206,7 @@
         <v>64</v>
       </c>
       <c r="F25" t="s">
-        <v>244</v>
+        <v>274</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -2086,7 +2226,7 @@
         <v>66</v>
       </c>
       <c r="F26" t="s">
-        <v>245</v>
+        <v>275</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -2106,7 +2246,7 @@
         <v>69</v>
       </c>
       <c r="F27" t="s">
-        <v>246</v>
+        <v>276</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -2126,7 +2266,7 @@
         <v>71</v>
       </c>
       <c r="F28" t="s">
-        <v>247</v>
+        <v>277</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -2146,7 +2286,7 @@
         <v>73</v>
       </c>
       <c r="F29" t="s">
-        <v>248</v>
+        <v>278</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -2166,7 +2306,7 @@
         <v>76</v>
       </c>
       <c r="F30" t="s">
-        <v>249</v>
+        <v>279</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -2186,7 +2326,7 @@
         <v>77</v>
       </c>
       <c r="F31" t="s">
-        <v>250</v>
+        <v>280</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -2206,7 +2346,7 @@
         <v>82</v>
       </c>
       <c r="F32" t="s">
-        <v>251</v>
+        <v>281</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -2226,7 +2366,7 @@
         <v>84</v>
       </c>
       <c r="F33" t="s">
-        <v>252</v>
+        <v>282</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -2246,7 +2386,7 @@
         <v>86</v>
       </c>
       <c r="F34" t="s">
-        <v>253</v>
+        <v>283</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -2266,7 +2406,7 @@
         <v>88</v>
       </c>
       <c r="F35" t="s">
-        <v>254</v>
+        <v>284</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -2286,7 +2426,7 @@
         <v>90</v>
       </c>
       <c r="F36" t="s">
-        <v>255</v>
+        <v>285</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -2306,7 +2446,7 @@
         <v>93</v>
       </c>
       <c r="F37" t="s">
-        <v>256</v>
+        <v>286</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -2326,7 +2466,7 @@
         <v>95</v>
       </c>
       <c r="F38" t="s">
-        <v>257</v>
+        <v>287</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -2346,7 +2486,7 @@
         <v>97</v>
       </c>
       <c r="F39" t="s">
-        <v>258</v>
+        <v>288</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -2366,7 +2506,7 @@
         <v>99</v>
       </c>
       <c r="F40" t="s">
-        <v>259</v>
+        <v>289</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -2386,7 +2526,7 @@
         <v>101</v>
       </c>
       <c r="F41" t="s">
-        <v>260</v>
+        <v>290</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -2406,7 +2546,7 @@
         <v>103</v>
       </c>
       <c r="F42" t="s">
-        <v>261</v>
+        <v>291</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -2426,7 +2566,7 @@
         <v>105</v>
       </c>
       <c r="F43" t="s">
-        <v>262</v>
+        <v>292</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -2446,7 +2586,7 @@
         <v>107</v>
       </c>
       <c r="F44" t="s">
-        <v>263</v>
+        <v>293</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -2466,7 +2606,7 @@
         <v>109</v>
       </c>
       <c r="F45" t="s">
-        <v>264</v>
+        <v>294</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -2486,7 +2626,7 @@
         <v>111</v>
       </c>
       <c r="F46" t="s">
-        <v>265</v>
+        <v>295</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -2506,7 +2646,7 @@
         <v>115</v>
       </c>
       <c r="F47" t="s">
-        <v>266</v>
+        <v>296</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -2526,7 +2666,7 @@
         <v>116</v>
       </c>
       <c r="F48" t="s">
-        <v>267</v>
+        <v>297</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -2546,7 +2686,7 @@
         <v>118</v>
       </c>
       <c r="F49" t="s">
-        <v>268</v>
+        <v>298</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -2566,7 +2706,7 @@
         <v>120</v>
       </c>
       <c r="F50" t="s">
-        <v>269</v>
+        <v>299</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -2586,7 +2726,7 @@
         <v>122</v>
       </c>
       <c r="F51" t="s">
-        <v>270</v>
+        <v>300</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -2606,7 +2746,7 @@
         <v>125</v>
       </c>
       <c r="F52" t="s">
-        <v>271</v>
+        <v>301</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -2626,7 +2766,7 @@
         <v>127</v>
       </c>
       <c r="F53" t="s">
-        <v>272</v>
+        <v>302</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -2646,7 +2786,7 @@
         <v>129</v>
       </c>
       <c r="F54" t="s">
-        <v>273</v>
+        <v>303</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -2666,7 +2806,7 @@
         <v>131</v>
       </c>
       <c r="F55" t="s">
-        <v>274</v>
+        <v>304</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
@@ -2686,7 +2826,7 @@
         <v>133</v>
       </c>
       <c r="F56" t="s">
-        <v>275</v>
+        <v>305</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
@@ -2706,7 +2846,7 @@
         <v>138</v>
       </c>
       <c r="F57" t="s">
-        <v>276</v>
+        <v>306</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -2726,7 +2866,7 @@
         <v>140</v>
       </c>
       <c r="F58" t="s">
-        <v>277</v>
+        <v>307</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -2746,7 +2886,7 @@
         <v>142</v>
       </c>
       <c r="F59" t="s">
-        <v>278</v>
+        <v>308</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -2766,7 +2906,7 @@
         <v>144</v>
       </c>
       <c r="F60" t="s">
-        <v>279</v>
+        <v>309</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
@@ -2786,7 +2926,7 @@
         <v>146</v>
       </c>
       <c r="F61" t="s">
-        <v>280</v>
+        <v>310</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
@@ -2806,7 +2946,7 @@
         <v>151</v>
       </c>
       <c r="F62" t="s">
-        <v>281</v>
+        <v>311</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
@@ -2826,7 +2966,7 @@
         <v>153</v>
       </c>
       <c r="F63" t="s">
-        <v>282</v>
+        <v>312</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -2846,7 +2986,7 @@
         <v>155</v>
       </c>
       <c r="F64" t="s">
-        <v>283</v>
+        <v>313</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
@@ -2866,7 +3006,7 @@
         <v>157</v>
       </c>
       <c r="F65" t="s">
-        <v>284</v>
+        <v>314</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -2886,7 +3026,7 @@
         <v>159</v>
       </c>
       <c r="F66" t="s">
-        <v>285</v>
+        <v>315</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -2906,7 +3046,7 @@
         <v>161</v>
       </c>
       <c r="F67" t="s">
-        <v>286</v>
+        <v>316</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
@@ -2926,7 +3066,7 @@
         <v>163</v>
       </c>
       <c r="F68" t="s">
-        <v>287</v>
+        <v>317</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
@@ -2946,7 +3086,7 @@
         <v>165</v>
       </c>
       <c r="F69" t="s">
-        <v>288</v>
+        <v>318</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
@@ -2966,7 +3106,7 @@
         <v>168</v>
       </c>
       <c r="F70" t="s">
-        <v>289</v>
+        <v>319</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
@@ -2986,7 +3126,7 @@
         <v>170</v>
       </c>
       <c r="F71" t="s">
-        <v>290</v>
+        <v>320</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
@@ -3006,7 +3146,7 @@
         <v>176</v>
       </c>
       <c r="F72" t="s">
-        <v>291</v>
+        <v>321</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
@@ -3026,7 +3166,7 @@
         <v>178</v>
       </c>
       <c r="F73" t="s">
-        <v>292</v>
+        <v>322</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
@@ -3046,7 +3186,7 @@
         <v>180</v>
       </c>
       <c r="F74" t="s">
-        <v>293</v>
+        <v>323</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
@@ -3066,7 +3206,7 @@
         <v>182</v>
       </c>
       <c r="F75" t="s">
-        <v>294</v>
+        <v>324</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
@@ -3086,7 +3226,7 @@
         <v>184</v>
       </c>
       <c r="F76" t="s">
-        <v>295</v>
+        <v>325</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
@@ -3106,7 +3246,7 @@
         <v>188</v>
       </c>
       <c r="F77" t="s">
-        <v>296</v>
+        <v>326</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
@@ -3126,7 +3266,7 @@
         <v>190</v>
       </c>
       <c r="F78" t="s">
-        <v>297</v>
+        <v>327</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
@@ -3146,7 +3286,7 @@
         <v>192</v>
       </c>
       <c r="F79" t="s">
-        <v>298</v>
+        <v>328</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
@@ -3166,7 +3306,7 @@
         <v>194</v>
       </c>
       <c r="F80" t="s">
-        <v>299</v>
+        <v>329</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
@@ -3186,7 +3326,7 @@
         <v>196</v>
       </c>
       <c r="F81" t="s">
-        <v>300</v>
+        <v>330</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
@@ -3206,7 +3346,7 @@
         <v>201</v>
       </c>
       <c r="F82" t="s">
-        <v>301</v>
+        <v>331</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
@@ -3226,7 +3366,7 @@
         <v>203</v>
       </c>
       <c r="F83" t="s">
-        <v>302</v>
+        <v>332</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
@@ -3246,7 +3386,7 @@
         <v>205</v>
       </c>
       <c r="F84" t="s">
-        <v>303</v>
+        <v>333</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
@@ -3266,7 +3406,7 @@
         <v>207</v>
       </c>
       <c r="F85" t="s">
-        <v>304</v>
+        <v>334</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
@@ -3286,7 +3426,7 @@
         <v>209</v>
       </c>
       <c r="F86" t="s">
-        <v>305</v>
+        <v>335</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
@@ -3306,7 +3446,7 @@
         <v>212</v>
       </c>
       <c r="F87" t="s">
-        <v>306</v>
+        <v>336</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
@@ -3326,7 +3466,7 @@
         <v>214</v>
       </c>
       <c r="F88" t="s">
-        <v>307</v>
+        <v>337</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
@@ -3346,7 +3486,7 @@
         <v>216</v>
       </c>
       <c r="F89" t="s">
-        <v>308</v>
+        <v>338</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
@@ -3366,7 +3506,7 @@
         <v>218</v>
       </c>
       <c r="F90" t="s">
-        <v>309</v>
+        <v>339</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
@@ -3386,12 +3526,328 @@
         <v>220</v>
       </c>
       <c r="F91" t="s">
-        <v>310</v>
+        <v>340</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{79E7101D-B434-4C34-92BE-2A6613F72505}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FA760DC-DD1E-41E7-A267-551CE2563A29}">
+  <dimension ref="A1:E26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.625" customWidth="1"/>
+    <col min="2" max="2" width="11.75" customWidth="1"/>
+    <col min="3" max="3" width="22.5" customWidth="1"/>
+    <col min="4" max="4" width="12.5" customWidth="1"/>
+    <col min="5" max="5" width="18.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B3" t="s">
+        <v>224</v>
+      </c>
+      <c r="C3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B4" t="s">
+        <v>224</v>
+      </c>
+      <c r="C4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>223</v>
+      </c>
+      <c r="B5" t="s">
+        <v>224</v>
+      </c>
+      <c r="C5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>223</v>
+      </c>
+      <c r="B6" t="s">
+        <v>224</v>
+      </c>
+      <c r="C6" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>223</v>
+      </c>
+      <c r="B7" t="s">
+        <v>224</v>
+      </c>
+      <c r="C7" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>223</v>
+      </c>
+      <c r="B8" t="s">
+        <v>224</v>
+      </c>
+      <c r="C8" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>223</v>
+      </c>
+      <c r="B9" t="s">
+        <v>224</v>
+      </c>
+      <c r="C9" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>223</v>
+      </c>
+      <c r="B10" t="s">
+        <v>224</v>
+      </c>
+      <c r="C10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>223</v>
+      </c>
+      <c r="B11" t="s">
+        <v>233</v>
+      </c>
+      <c r="C11" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>223</v>
+      </c>
+      <c r="B12" t="s">
+        <v>233</v>
+      </c>
+      <c r="C12" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>223</v>
+      </c>
+      <c r="B13" t="s">
+        <v>233</v>
+      </c>
+      <c r="C13" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>223</v>
+      </c>
+      <c r="B14" t="s">
+        <v>233</v>
+      </c>
+      <c r="C14" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>223</v>
+      </c>
+      <c r="B15" t="s">
+        <v>233</v>
+      </c>
+      <c r="C15" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>223</v>
+      </c>
+      <c r="B16" t="s">
+        <v>233</v>
+      </c>
+      <c r="C16" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>223</v>
+      </c>
+      <c r="B17" t="s">
+        <v>240</v>
+      </c>
+      <c r="C17" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>223</v>
+      </c>
+      <c r="B18" t="s">
+        <v>240</v>
+      </c>
+      <c r="C18" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>223</v>
+      </c>
+      <c r="B19" t="s">
+        <v>240</v>
+      </c>
+      <c r="C19" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>223</v>
+      </c>
+      <c r="B20" t="s">
+        <v>240</v>
+      </c>
+      <c r="C20" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>223</v>
+      </c>
+      <c r="B21" t="s">
+        <v>240</v>
+      </c>
+      <c r="C21" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>223</v>
+      </c>
+      <c r="B22" t="s">
+        <v>240</v>
+      </c>
+      <c r="C22" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>223</v>
+      </c>
+      <c r="B23" t="s">
+        <v>240</v>
+      </c>
+      <c r="C23" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>223</v>
+      </c>
+      <c r="B24" t="s">
+        <v>247</v>
+      </c>
+      <c r="C24" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>223</v>
+      </c>
+      <c r="B25" t="s">
+        <v>247</v>
+      </c>
+      <c r="C25" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>223</v>
+      </c>
+      <c r="B26" t="s">
+        <v>247</v>
+      </c>
+      <c r="C26" t="s">
+        <v>250</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>